<commit_message>
Fin, a falta de revisión
</commit_message>
<xml_diff>
--- a/PR1.xlsx
+++ b/PR1.xlsx
@@ -16,12 +16,12 @@
     <sheet name="PROGRESO" sheetId="9" r:id="rId7"/>
     <sheet name="Hoja1" sheetId="14" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="49">
   <si>
     <t>Operaciones</t>
   </si>
@@ -125,54 +125,6 @@
     <t>Speed-Up por sobreasignacion</t>
   </si>
   <si>
-    <t>Talla 12400</t>
-  </si>
-  <si>
-    <t>Talla 100</t>
-  </si>
-  <si>
-    <t>Talla 400</t>
-  </si>
-  <si>
-    <t>Talla 900</t>
-  </si>
-  <si>
-    <t>Talla 1400</t>
-  </si>
-  <si>
-    <t>Talla 2300</t>
-  </si>
-  <si>
-    <t>Talla 5100</t>
-  </si>
-  <si>
-    <t>Talla 88800</t>
-  </si>
-  <si>
-    <t>AW</t>
-  </si>
-  <si>
-    <t>AX</t>
-  </si>
-  <si>
-    <t>AQ</t>
-  </si>
-  <si>
-    <t>AR</t>
-  </si>
-  <si>
-    <t>AS</t>
-  </si>
-  <si>
-    <t>AT</t>
-  </si>
-  <si>
-    <t>AU</t>
-  </si>
-  <si>
-    <t>AV</t>
-  </si>
-  <si>
     <t>MOPS O0</t>
   </si>
   <si>
@@ -207,6 +159,15 @@
   </si>
   <si>
     <t>Talla:</t>
+  </si>
+  <si>
+    <t>Escalabilidad</t>
+  </si>
+  <si>
+    <t>Procesadores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tamaño </t>
   </si>
 </sst>
 </file>
@@ -409,7 +370,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -496,11 +456,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84526208"/>
-        <c:axId val="84528512"/>
+        <c:axId val="85128320"/>
+        <c:axId val="85136512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84526208"/>
+        <c:axId val="85128320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -522,19 +482,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84528512"/>
+        <c:crossAx val="85136512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84528512"/>
+        <c:axId val="85136512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -557,21 +516,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84526208"/>
+        <c:crossAx val="85128320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1094,11 +1051,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="535278336"/>
-        <c:axId val="535281024"/>
+        <c:axId val="3409408"/>
+        <c:axId val="3411328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="535278336"/>
+        <c:axId val="3409408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1127,12 +1084,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="535281024"/>
+        <c:crossAx val="3411328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="535281024"/>
+        <c:axId val="3411328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1162,7 +1119,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="535278336"/>
+        <c:crossAx val="3409408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1692,11 +1649,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="495451520"/>
-        <c:axId val="502346880"/>
+        <c:axId val="3469312"/>
+        <c:axId val="3471232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="495451520"/>
+        <c:axId val="3469312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1725,12 +1682,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="502346880"/>
+        <c:crossAx val="3471232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="502346880"/>
+        <c:axId val="3471232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1760,7 +1717,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="495451520"/>
+        <c:crossAx val="3469312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2285,11 +2242,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="336213120"/>
-        <c:axId val="336214656"/>
+        <c:axId val="3520768"/>
+        <c:axId val="3522944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="336213120"/>
+        <c:axId val="3520768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2318,12 +2275,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="336214656"/>
+        <c:crossAx val="3522944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="336214656"/>
+        <c:axId val="3522944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2353,7 +2310,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="336213120"/>
+        <c:crossAx val="3520768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2435,10 +2392,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$AQ$9:$AW$9</c:f>
+              <c:f>'Datos finales OMP Adecuados'!$AQ$9:$AV$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
@@ -2456,19 +2413,16 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12400</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$AQ$10:$AW$10</c:f>
+              <c:f>'Datos finales OMP Adecuados'!$AQ$10:$AV$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2485,9 +2439,6 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -2511,10 +2462,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$AQ$9:$AW$9</c:f>
+              <c:f>'Datos finales OMP Adecuados'!$AQ$9:$AV$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
@@ -2532,19 +2483,16 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12400</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$AQ$11:$AW$11</c:f>
+              <c:f>'Datos finales OMP Adecuados'!$AQ$11:$AV$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.25908328675237563</c:v>
                 </c:pt>
@@ -2562,9 +2510,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.0132435054235573</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.91842711769462704</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2587,10 +2532,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$AQ$9:$AW$9</c:f>
+              <c:f>'Datos finales OMP Adecuados'!$AQ$9:$AV$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
@@ -2608,19 +2553,16 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12400</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$AQ$12:$AW$12</c:f>
+              <c:f>'Datos finales OMP Adecuados'!$AQ$12:$AV$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>3.4318080852954243E-2</c:v>
                 </c:pt>
@@ -2638,9 +2580,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.95654492427468973</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.88553491141565022</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2663,10 +2602,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$AQ$9:$AW$9</c:f>
+              <c:f>'Datos finales OMP Adecuados'!$AQ$9:$AV$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
@@ -2684,19 +2623,16 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12400</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$AQ$13:$AW$13</c:f>
+              <c:f>'Datos finales OMP Adecuados'!$AQ$13:$AV$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>9.0224246671338475E-3</c:v>
                 </c:pt>
@@ -2714,9 +2650,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.66199233637468557</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.55636291028423746</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2739,10 +2672,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$AQ$9:$AW$9</c:f>
+              <c:f>'Datos finales OMP Adecuados'!$AQ$9:$AV$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
@@ -2760,19 +2693,16 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12400</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$AQ$14:$AW$14</c:f>
+              <c:f>'Datos finales OMP Adecuados'!$AQ$14:$AV$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>4.2342688007016007E-3</c:v>
                 </c:pt>
@@ -2790,9 +2720,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.58051032249760937</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.54508436162686269</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2815,10 +2742,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$AQ$9:$AW$9</c:f>
+              <c:f>'Datos finales OMP Adecuados'!$AQ$9:$AV$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
@@ -2836,19 +2763,16 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12400</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$AQ$15:$AW$15</c:f>
+              <c:f>'Datos finales OMP Adecuados'!$AQ$15:$AV$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>8.688170591807815E-4</c:v>
                 </c:pt>
@@ -2866,9 +2790,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.25933464199128892</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.3334187692711359</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2883,11 +2804,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="336251520"/>
-        <c:axId val="336253312"/>
+        <c:axId val="3556096"/>
+        <c:axId val="3558016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="336251520"/>
+        <c:axId val="3556096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2916,12 +2837,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="336253312"/>
+        <c:crossAx val="3558016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="336253312"/>
+        <c:axId val="3558016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2951,7 +2872,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="336251520"/>
+        <c:crossAx val="3556096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3476,11 +3397,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="346706688"/>
-        <c:axId val="346708224"/>
+        <c:axId val="3599744"/>
+        <c:axId val="3741184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="346706688"/>
+        <c:axId val="3599744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3509,12 +3430,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="346708224"/>
+        <c:crossAx val="3741184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="346708224"/>
+        <c:axId val="3741184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3544,7 +3465,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="346706688"/>
+        <c:crossAx val="3599744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4069,11 +3990,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="346740992"/>
-        <c:axId val="347738112"/>
+        <c:axId val="3782528"/>
+        <c:axId val="3801088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="346740992"/>
+        <c:axId val="3782528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4102,12 +4023,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="347738112"/>
+        <c:crossAx val="3801088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="347738112"/>
+        <c:axId val="3801088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4137,7 +4058,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="346740992"/>
+        <c:crossAx val="3782528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4662,11 +4583,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="347774976"/>
-        <c:axId val="347776512"/>
+        <c:axId val="3842432"/>
+        <c:axId val="3844352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="347774976"/>
+        <c:axId val="3842432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4695,12 +4616,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="347776512"/>
+        <c:crossAx val="3844352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="347776512"/>
+        <c:axId val="3844352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4730,7 +4651,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="347774976"/>
+        <c:crossAx val="3842432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5219,11 +5140,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="351999488"/>
-        <c:axId val="352001024"/>
+        <c:axId val="4213376"/>
+        <c:axId val="4215552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="351999488"/>
+        <c:axId val="4213376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5252,12 +5173,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="352001024"/>
+        <c:crossAx val="4215552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="352001024"/>
+        <c:axId val="4215552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5287,7 +5208,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="351999488"/>
+        <c:crossAx val="4213376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5781,11 +5702,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="352029312"/>
-        <c:axId val="352039296"/>
+        <c:axId val="4272896"/>
+        <c:axId val="4274816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="352029312"/>
+        <c:axId val="4272896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5814,12 +5735,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="352039296"/>
+        <c:crossAx val="4274816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="352039296"/>
+        <c:axId val="4274816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5849,7 +5770,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="352029312"/>
+        <c:crossAx val="4272896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5895,9 +5816,14 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Escalabilidad -O0</a:t>
+              <a:rPr lang="es-ES"/>
+              <a:t>Escalabilidad</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="es-ES" baseline="0"/>
+              <a:t> -O2</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -5906,27 +5832,53 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.7443493118625093E-2"/>
+          <c:y val="0.14844027777777777"/>
+          <c:w val="0.86434811914171261"/>
+          <c:h val="0.68837638888888886"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="7"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos finales OMP Adecuados'!$C$66</c:f>
+              <c:f>'Datos finales OMP Adecuados'!$D$84</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Talla 100</c:v>
+                  <c:v>Eficiencia</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$65:$H$65</c:f>
+              <c:f>'Datos finales OMP Adecuados'!$E$80:$I$80</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5950,7 +5902,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$66:$H$66</c:f>
+              <c:f>'Datos finales OMP Adecuados'!$E$84:$I$84</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5958,464 +5910,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.36792083088379385</c:v>
+                  <c:v>0.85</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1113714556886938</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.9115749643322378E-2</c:v>
+                  <c:v>0.48</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2898461115691123E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Datos finales OMP Adecuados'!$C$67</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Talla 400</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$65:$H$65</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$67:$H$67</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.54366387691267226</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.43764177479357591</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.18829787234042553</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.9717794455126227E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Datos finales OMP Adecuados'!$C$68</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Talla 900</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$65:$H$65</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$68:$H$68</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.72897567209115466</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.54181177147791049</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.33535075530853642</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.24504865111132809</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Datos finales OMP Adecuados'!$C$69</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Talla 1400</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$65:$H$65</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$69:$H$69</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.034439721572431</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.78574291967323229</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.51069785456081873</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.40264776752501191</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Datos finales OMP Adecuados'!$C$70</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Talla 2300</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$65:$H$65</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$70:$H$70</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.93650863170188703</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.74080896151514286</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.50218020980115863</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.44196072554906207</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Datos finales OMP Adecuados'!$C$71</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Talla 5100</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$65:$H$65</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$71:$H$71</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.94412216699420082</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.84780640050436873</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.59052418680620455</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.54243097202989976</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Datos finales OMP Adecuados'!$C$72</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Talla 12400</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$65:$H$65</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$72:$H$72</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.068205147354846</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.80766383159997135</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.53530930135089871</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.51304319393858433</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Datos finales OMP Adecuados'!$C$73</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Talla 88800</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$65:$H$65</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$73:$H$73</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.91109985103178226</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.82126597234726484</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.70497287194209812</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.68717445123068088</c:v>
+                  <c:v>0.42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6430,11 +5934,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="353851264"/>
-        <c:axId val="353852800"/>
+        <c:axId val="4316160"/>
+        <c:axId val="4322432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="353851264"/>
+        <c:axId val="4316160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6463,12 +5967,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353852800"/>
+        <c:crossAx val="4322432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="353852800"/>
+        <c:axId val="4322432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6485,7 +5989,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="es-ES"/>
+                  <a:rPr lang="en-US"/>
                   <a:t>Eficiencia</a:t>
                 </a:r>
               </a:p>
@@ -6498,15 +6002,31 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353851264"/>
+        <c:crossAx val="4316160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.60316889273210039"/>
+          <c:y val="0.18054583333333329"/>
+          <c:w val="0.12030017731320224"/>
+          <c:h val="6.3792500000000002E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -6550,7 +6070,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6637,11 +6156,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="185956608"/>
-        <c:axId val="186286848"/>
+        <c:axId val="86697472"/>
+        <c:axId val="87470080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="185956608"/>
+        <c:axId val="86697472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6668,19 +6187,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186286848"/>
+        <c:crossAx val="87470080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="186286848"/>
+        <c:axId val="87470080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6756,675 +6274,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185956608"/>
+        <c:crossAx val="86697472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-ES"/>
-              <a:t>Escalabilidad</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="es-ES" baseline="0"/>
-              <a:t> -O2</a:t>
-            </a:r>
-            <a:endParaRPr lang="es-ES"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Datos finales OMP Adecuados'!$C$76</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Talla 100</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$75:$H$75</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$76:$H$76</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.25908328675237563</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.4318080852954243E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.0224246671338475E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.2342688007016007E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Datos finales OMP Adecuados'!$C$77</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Talla 400</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$75:$H$75</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$77:$H$77</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.4340626178800453</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.24776074412195334</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.3787208015378339E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.4201828536101105E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Datos finales OMP Adecuados'!$C$78</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Talla 900</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$75:$H$75</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$78:$H$78</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.5837386664148092</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.45768846267772506</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.18458442838370565</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.11894967282525019</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Datos finales OMP Adecuados'!$C$79</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Talla 1400</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$75:$H$75</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$79:$H$79</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.85587103802812114</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.65277056501869546</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.39882866208355372</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.24774814727215388</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Datos finales OMP Adecuados'!$C$80</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Talla 2300</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$75:$H$75</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$80:$H$80</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.74037112654474202</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.65561263492645938</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.42923494259316725</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.32590042332626529</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Datos finales OMP Adecuados'!$C$81</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Talla 5100</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$75:$H$75</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$81:$H$81</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0132435054235573</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.95654492427468973</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.66199233637468557</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.58051032249760937</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Datos finales OMP Adecuados'!$C$82</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Talla 12400</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$75:$H$75</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$82:$H$82</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.91842711769462704</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.88553491141565022</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.55636291028423746</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.54508436162686269</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Datos finales OMP Adecuados'!$C$83</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Talla 88800</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$75:$H$75</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Datos finales OMP Adecuados'!$D$83:$H$83</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.90940071715024406</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.75528135029279431</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.72884005664714269</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.69801573514423099</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="452400256"/>
-        <c:axId val="452401792"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="452400256"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Procesadores</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="452401792"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="452401792"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Eficiencia</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="452400256"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7561,11 +6423,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="209995264"/>
-        <c:axId val="210002304"/>
+        <c:axId val="87092608"/>
+        <c:axId val="87115264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="209995264"/>
+        <c:axId val="87092608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7593,12 +6455,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210002304"/>
+        <c:crossAx val="87115264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="210002304"/>
+        <c:axId val="87115264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7627,7 +6489,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209995264"/>
+        <c:crossAx val="87092608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7678,7 +6540,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7771,11 +6632,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="213744640"/>
-        <c:axId val="213757312"/>
+        <c:axId val="98178944"/>
+        <c:axId val="98197504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="213744640"/>
+        <c:axId val="98178944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7797,19 +6658,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213757312"/>
+        <c:crossAx val="98197504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="213757312"/>
+        <c:axId val="98197504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7832,21 +6692,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213744640"/>
+        <c:crossAx val="98178944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7891,7 +6749,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7984,11 +6841,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="214746624"/>
-        <c:axId val="214770816"/>
+        <c:axId val="182210944"/>
+        <c:axId val="182212864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="214746624"/>
+        <c:axId val="182210944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8010,19 +6867,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214770816"/>
+        <c:crossAx val="182212864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="214770816"/>
+        <c:axId val="182212864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8045,21 +6901,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214746624"/>
+        <c:crossAx val="182210944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8541,11 +7395,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="306625152"/>
-        <c:axId val="308839168"/>
+        <c:axId val="3211264"/>
+        <c:axId val="3213184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="306625152"/>
+        <c:axId val="3211264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8574,12 +7428,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="308839168"/>
+        <c:crossAx val="3213184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="308839168"/>
+        <c:axId val="3213184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8609,7 +7463,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="306625152"/>
+        <c:crossAx val="3211264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9098,11 +7952,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="333080832"/>
-        <c:axId val="335179776"/>
+        <c:axId val="3246336"/>
+        <c:axId val="3260800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="333080832"/>
+        <c:axId val="3246336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9131,12 +7985,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="335179776"/>
+        <c:crossAx val="3260800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="335179776"/>
+        <c:axId val="3260800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9166,7 +8020,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="333080832"/>
+        <c:crossAx val="3246336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9655,11 +8509,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="412391296"/>
-        <c:axId val="412524928"/>
+        <c:axId val="3298048"/>
+        <c:axId val="3299968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="412391296"/>
+        <c:axId val="3298048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9688,12 +8542,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412524928"/>
+        <c:crossAx val="3299968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="412524928"/>
+        <c:axId val="3299968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9728,7 +8582,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412391296"/>
+        <c:crossAx val="3298048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10222,11 +9076,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="431419392"/>
-        <c:axId val="431420928"/>
+        <c:axId val="3619840"/>
+        <c:axId val="3622016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="431419392"/>
+        <c:axId val="3619840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10255,12 +9109,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="431420928"/>
+        <c:crossAx val="3622016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="431420928"/>
+        <c:axId val="3622016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10290,7 +9144,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="431419392"/>
+        <c:crossAx val="3619840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10705,16 +9559,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>407333</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>94129</xdr:rowOff>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>472532</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>65603</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>44</xdr:col>
-      <xdr:colOff>491598</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>74629</xdr:rowOff>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>34637</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>46103</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10897,48 +9751,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>598712</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>70759</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>855647</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>180417</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>257153</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>51259</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="17" name="16 Gráfico"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>362588</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>90769</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>704588</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>71269</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>514088</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>160917</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10953,7 +9775,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -12718,7 +11540,7 @@
     </row>
     <row r="33" spans="14:22" x14ac:dyDescent="0.25">
       <c r="N33" s="1" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="O33" s="1">
         <f t="shared" ref="O33:V33" si="5">O$32/(D2/1000000)/10^6</f>
@@ -12755,7 +11577,7 @@
     </row>
     <row r="34" spans="14:22" x14ac:dyDescent="0.25">
       <c r="N34" s="1" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="O34" s="1">
         <f t="shared" ref="O34:V34" si="6">O$32/(D8/1000000)/10^6</f>
@@ -15112,8 +13934,8 @@
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:AI25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17345,15 +16167,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX83"/>
+  <dimension ref="A1:AX84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q93" sqref="Q93"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X78" sqref="X78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.42578125" customWidth="1"/>
     <col min="13" max="13" width="31.140625" bestFit="1" customWidth="1"/>
@@ -19827,7 +18650,7 @@
     </row>
     <row r="49" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C49" s="1" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="D49" s="1">
         <f t="shared" ref="D49:K49" si="20">D1*100</f>
@@ -20853,47 +19676,7 @@
       <c r="Z63" s="1"/>
       <c r="AA63" s="1"/>
     </row>
-    <row r="64" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="D64">
-        <v>2</v>
-      </c>
-      <c r="E64">
-        <v>3</v>
-      </c>
-      <c r="F64">
-        <v>4</v>
-      </c>
-      <c r="G64">
-        <v>5</v>
-      </c>
-      <c r="H64">
-        <v>6</v>
-      </c>
-      <c r="I64">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="65" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="D65">
-        <f>N65</f>
-        <v>1</v>
-      </c>
-      <c r="E65">
-        <f>O65</f>
-        <v>2</v>
-      </c>
-      <c r="F65">
-        <v>4</v>
-      </c>
-      <c r="G65">
-        <v>8</v>
-      </c>
-      <c r="H65">
-        <v>12</v>
-      </c>
-      <c r="I65">
-        <v>24</v>
-      </c>
+    <row r="65" spans="4:27" x14ac:dyDescent="0.25">
       <c r="M65" s="1" t="s">
         <v>33</v>
       </c>
@@ -20929,63 +19712,33 @@
       <c r="Z65" s="1"/>
       <c r="AA65" s="1"/>
     </row>
-    <row r="66" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>44</v>
-      </c>
-      <c r="C66" t="s">
-        <v>35</v>
-      </c>
-      <c r="D66">
-        <f ca="1">INDIRECT($B66&amp;D$64)</f>
-        <v>1</v>
-      </c>
-      <c r="E66">
-        <f ca="1">INDIRECT($B66&amp;E$64)</f>
-        <v>0.36792083088379385</v>
-      </c>
-      <c r="F66">
-        <f ca="1">INDIRECT($B66&amp;F$64)</f>
-        <v>0.1113714556886938</v>
-      </c>
-      <c r="G66">
-        <f ca="1">INDIRECT($B66&amp;G$64)</f>
-        <v>2.9115749643322378E-2</v>
-      </c>
-      <c r="H66">
-        <f t="shared" ref="F66:I66" ca="1" si="37">INDIRECT($B66&amp;H$64)</f>
-        <v>1.2898461115691123E-2</v>
-      </c>
-      <c r="I66">
-        <f t="shared" ca="1" si="37"/>
-        <v>3.1477383227710154E-3</v>
-      </c>
+    <row r="66" spans="4:27" x14ac:dyDescent="0.25">
       <c r="M66" s="1" t="str">
         <f>M10</f>
         <v>1 procesador</v>
       </c>
       <c r="N66" s="1">
-        <f t="shared" ref="N66:S71" si="38">$N$10/N10</f>
+        <f t="shared" ref="N66:S71" si="37">$N$10/N10</f>
         <v>1</v>
       </c>
       <c r="O66" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>1.0233004910969938</v>
       </c>
       <c r="P66" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>1.0091938339206055</v>
       </c>
       <c r="Q66" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>1.0173816921368732</v>
       </c>
       <c r="R66" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>1.0029483858105226</v>
       </c>
       <c r="S66" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>0.99447831148285226</v>
       </c>
       <c r="U66" s="1"/>
@@ -20996,39 +19749,9 @@
       <c r="Z66" s="1"/>
       <c r="AA66" s="1"/>
     </row>
-    <row r="67" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>45</v>
-      </c>
-      <c r="C67" t="s">
-        <v>36</v>
-      </c>
-      <c r="D67">
-        <f t="shared" ref="D67:I73" ca="1" si="39">INDIRECT($B67&amp;D$64)</f>
-        <v>1</v>
-      </c>
-      <c r="E67">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.54366387691267226</v>
-      </c>
-      <c r="F67">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.43764177479357591</v>
-      </c>
-      <c r="G67">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.18829787234042553</v>
-      </c>
-      <c r="H67">
-        <f t="shared" ca="1" si="39"/>
-        <v>9.9717794455126227E-2</v>
-      </c>
-      <c r="I67">
-        <f t="shared" ca="1" si="39"/>
-        <v>2.6332814675292766E-2</v>
-      </c>
+    <row r="67" spans="4:27" x14ac:dyDescent="0.25">
       <c r="M67" s="1" t="str">
-        <f t="shared" ref="M67:M71" si="40">M11</f>
+        <f t="shared" ref="M67:M71" si="38">M11</f>
         <v>2 procesadores</v>
       </c>
       <c r="N67" s="1">
@@ -21036,23 +19759,23 @@
         <v>1.8368542353892541</v>
       </c>
       <c r="O67" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>2.1412360036639377</v>
       </c>
       <c r="P67" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>1.8077699409822794</v>
       </c>
       <c r="Q67" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>1.8192553190049807</v>
       </c>
       <c r="R67" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>1.3418266789594699</v>
       </c>
       <c r="S67" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>0.87956011902634701</v>
       </c>
       <c r="U67" s="1"/>
@@ -21063,39 +19786,9 @@
       <c r="Z67" s="1"/>
       <c r="AA67" s="1"/>
     </row>
-    <row r="68" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>46</v>
-      </c>
-      <c r="C68" t="s">
-        <v>37</v>
-      </c>
-      <c r="D68">
-        <f t="shared" ca="1" si="39"/>
-        <v>1</v>
-      </c>
-      <c r="E68">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.72897567209115466</v>
-      </c>
-      <c r="F68">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.54181177147791049</v>
-      </c>
-      <c r="G68">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.33535075530853642</v>
-      </c>
-      <c r="H68">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.24504865111132809</v>
-      </c>
-      <c r="I68">
-        <f t="shared" ca="1" si="39"/>
-        <v>8.448787340226914E-2</v>
-      </c>
+    <row r="68" spans="4:27" x14ac:dyDescent="0.25">
       <c r="M68" s="1" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>4 procesadores</v>
       </c>
       <c r="N68" s="1">
@@ -21107,19 +19800,19 @@
         <v>3.5060426575045063</v>
       </c>
       <c r="P68" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>3.5320382304493232</v>
       </c>
       <c r="Q68" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>2.8296523528142741</v>
       </c>
       <c r="R68" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>1.7147551709932056</v>
       </c>
       <c r="S68" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>0.76509389274439066</v>
       </c>
       <c r="U68" s="1"/>
@@ -21130,39 +19823,9 @@
       <c r="Z68" s="1"/>
       <c r="AA68" s="1"/>
     </row>
-    <row r="69" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>47</v>
-      </c>
-      <c r="C69" t="s">
-        <v>38</v>
-      </c>
-      <c r="D69">
-        <f t="shared" ca="1" si="39"/>
-        <v>1</v>
-      </c>
-      <c r="E69">
-        <f t="shared" ca="1" si="39"/>
-        <v>1.034439721572431</v>
-      </c>
-      <c r="F69">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.78574291967323229</v>
-      </c>
-      <c r="G69">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.51069785456081873</v>
-      </c>
-      <c r="H69">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.40264776752501191</v>
-      </c>
-      <c r="I69">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.16027213500229837</v>
-      </c>
+    <row r="69" spans="4:27" x14ac:dyDescent="0.25">
       <c r="M69" s="1" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>8 procesadores</v>
       </c>
       <c r="N69" s="1">
@@ -21178,15 +19841,15 @@
         <v>4.0838903277568699</v>
       </c>
       <c r="Q69" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>2.8697765857417452</v>
       </c>
       <c r="R69" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>1.5057430729279611</v>
       </c>
       <c r="S69" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>0.58912110221432301</v>
       </c>
       <c r="U69" s="1"/>
@@ -21197,39 +19860,9 @@
       <c r="Z69" s="1"/>
       <c r="AA69" s="1"/>
     </row>
-    <row r="70" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>48</v>
-      </c>
-      <c r="C70" t="s">
-        <v>39</v>
-      </c>
-      <c r="D70">
-        <f t="shared" ca="1" si="39"/>
-        <v>1</v>
-      </c>
-      <c r="E70">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.93650863170188703</v>
-      </c>
-      <c r="F70">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.74080896151514286</v>
-      </c>
-      <c r="G70">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.50218020980115863</v>
-      </c>
-      <c r="H70">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.44196072554906207</v>
-      </c>
-      <c r="I70">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.21510281752718188</v>
-      </c>
+    <row r="70" spans="4:27" x14ac:dyDescent="0.25">
       <c r="M70" s="1" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>12 procesadores</v>
       </c>
       <c r="N70" s="1">
@@ -21249,11 +19882,11 @@
         <v>2.9425304589032906</v>
       </c>
       <c r="R70" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>1.4025983035989771</v>
       </c>
       <c r="S70" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>0.49394997560205517</v>
       </c>
       <c r="U70" s="1"/>
@@ -21264,39 +19897,9 @@
       <c r="Z70" s="1"/>
       <c r="AA70" s="1"/>
     </row>
-    <row r="71" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
-        <v>49</v>
-      </c>
-      <c r="C71" t="s">
-        <v>40</v>
-      </c>
-      <c r="D71">
-        <f t="shared" ca="1" si="39"/>
-        <v>1</v>
-      </c>
-      <c r="E71">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.94412216699420082</v>
-      </c>
-      <c r="F71">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.84780640050436873</v>
-      </c>
-      <c r="G71">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.59052418680620455</v>
-      </c>
-      <c r="H71">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.54243097202989976</v>
-      </c>
-      <c r="I71">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.3365627199047429</v>
-      </c>
+    <row r="71" spans="4:27" x14ac:dyDescent="0.25">
       <c r="M71" s="1" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>24 procesadores</v>
       </c>
       <c r="N71" s="1">
@@ -21320,7 +19923,7 @@
         <v>0.76868543590637139</v>
       </c>
       <c r="S71" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>0.318333457790417</v>
       </c>
       <c r="U71" s="1"/>
@@ -21331,367 +19934,229 @@
       <c r="Z71" s="1"/>
       <c r="AA71" s="1"/>
     </row>
-    <row r="72" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
-        <v>42</v>
-      </c>
-      <c r="C72" t="s">
-        <v>34</v>
-      </c>
-      <c r="D72">
-        <f t="shared" ca="1" si="39"/>
+    <row r="73" spans="4:27" x14ac:dyDescent="0.25">
+      <c r="E73" s="1">
         <v>1</v>
       </c>
-      <c r="E72">
-        <f t="shared" ca="1" si="39"/>
-        <v>1.068205147354846</v>
-      </c>
-      <c r="F72">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.80766383159997135</v>
-      </c>
-      <c r="G72">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.53530930135089871</v>
-      </c>
-      <c r="H72">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.51304319393858433</v>
-      </c>
-      <c r="I72">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.37958756735963256</v>
-      </c>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
     </row>
-    <row r="73" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>43</v>
-      </c>
-      <c r="C73" t="s">
-        <v>41</v>
-      </c>
-      <c r="D73">
-        <f t="shared" ca="1" si="39"/>
+    <row r="74" spans="4:27" x14ac:dyDescent="0.25">
+      <c r="E74" s="1">
+        <f>E73</f>
         <v>1</v>
       </c>
-      <c r="E73">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.91109985103178226</v>
-      </c>
-      <c r="F73">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.82126597234726484</v>
-      </c>
-      <c r="G73">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.70497287194209812</v>
-      </c>
-      <c r="H73">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.68717445123068088</v>
-      </c>
-      <c r="I73">
-        <f t="shared" ca="1" si="39"/>
-        <v>0.46414562061132453</v>
+      <c r="F74" s="1">
+        <f t="shared" ref="F74:J74" si="39">F73</f>
+        <v>0</v>
+      </c>
+      <c r="G74" s="1">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="H74" s="1">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="I74" s="1">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="J74" s="1">
+        <f t="shared" si="39"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="D74">
-        <v>10</v>
-      </c>
-      <c r="E74">
-        <v>11</v>
-      </c>
-      <c r="F74">
+    <row r="75" spans="4:27" x14ac:dyDescent="0.25">
+      <c r="E75" s="1">
+        <f>E73</f>
+        <v>1</v>
+      </c>
+      <c r="F75" s="1">
+        <f t="shared" ref="F75:I75" si="40">F73</f>
+        <v>0</v>
+      </c>
+      <c r="G75" s="1">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="H75" s="1">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="I75" s="1">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="J75" s="1">
+        <f t="shared" ref="J75" si="41">J73</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="4:27" x14ac:dyDescent="0.25">
+      <c r="E76" s="1">
+        <f>E73</f>
+        <v>1</v>
+      </c>
+      <c r="F76" s="1">
+        <f t="shared" ref="F76:I76" si="42">F73</f>
+        <v>0</v>
+      </c>
+      <c r="G76" s="1">
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+      <c r="H76" s="1">
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+      <c r="I76" s="1">
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+      <c r="J76" s="1">
+        <f t="shared" ref="J76" si="43">J73</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="4:27" x14ac:dyDescent="0.25">
+      <c r="E77" s="1">
+        <f>E73</f>
+        <v>1</v>
+      </c>
+      <c r="F77" s="1">
+        <f t="shared" ref="F77:I77" si="44">F73</f>
+        <v>0</v>
+      </c>
+      <c r="G77" s="1">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="H77" s="1">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="I77" s="1">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="J77" s="1">
+        <f t="shared" ref="J77" si="45">J73</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="4:27" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="80" spans="4:27" x14ac:dyDescent="0.25">
+      <c r="D80" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E80" s="1">
+        <v>1</v>
+      </c>
+      <c r="F80" s="1">
+        <v>2</v>
+      </c>
+      <c r="G80" s="1">
+        <v>4</v>
+      </c>
+      <c r="H80" s="1">
+        <v>8</v>
+      </c>
+      <c r="I80" s="1">
         <v>12</v>
       </c>
-      <c r="G74">
-        <v>13</v>
-      </c>
-      <c r="H74">
-        <v>14</v>
-      </c>
-      <c r="I74">
-        <v>15</v>
-      </c>
     </row>
-    <row r="75" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="D75">
-        <f>N65</f>
+    <row r="81" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D81" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E81" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F81" s="1">
+        <v>1400</v>
+      </c>
+      <c r="G81" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H81" s="1">
+        <v>2800</v>
+      </c>
+      <c r="I81" s="1">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="82" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E82" s="1">
+        <f>(19*E81*E81)/E80</f>
+        <v>19000000</v>
+      </c>
+      <c r="F82" s="1">
+        <f>(19*F81*F81)/F80</f>
+        <v>18620000</v>
+      </c>
+      <c r="G82" s="1">
+        <f>(19*G81*G81)/G80</f>
+        <v>19000000</v>
+      </c>
+      <c r="H82" s="1">
+        <f>(19*H81*H81)/H80</f>
+        <v>18620000</v>
+      </c>
+      <c r="I82" s="1">
+        <f>(19*I81*I81)/I80</f>
+        <v>19395833.333333332</v>
+      </c>
+    </row>
+    <row r="83" spans="4:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1">
+        <f>F82/E82</f>
+        <v>0.98</v>
+      </c>
+      <c r="G83" s="1">
+        <f>G82/F82</f>
+        <v>1.0204081632653061</v>
+      </c>
+      <c r="H83" s="1">
+        <f>H82/G82</f>
+        <v>0.98</v>
+      </c>
+      <c r="I83" s="1">
+        <f>I82/H82</f>
+        <v>1.0416666666666665</v>
+      </c>
+    </row>
+    <row r="84" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D84" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E84" s="1">
+        <f>1</f>
         <v>1</v>
       </c>
-      <c r="E75">
-        <f>O65</f>
-        <v>2</v>
-      </c>
-      <c r="F75">
-        <v>4</v>
-      </c>
-      <c r="G75">
-        <v>8</v>
-      </c>
-      <c r="H75">
-        <v>12</v>
-      </c>
-      <c r="I75">
-        <f>I65</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="76" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
-        <v>44</v>
-      </c>
-      <c r="C76" t="s">
-        <v>35</v>
-      </c>
-      <c r="D76">
-        <f ca="1">INDIRECT($B76&amp;D$74)</f>
-        <v>1</v>
-      </c>
-      <c r="E76">
-        <f t="shared" ref="E76:I76" ca="1" si="41">INDIRECT($B76&amp;E$74)</f>
-        <v>0.25908328675237563</v>
-      </c>
-      <c r="F76">
-        <f t="shared" ca="1" si="41"/>
-        <v>3.4318080852954243E-2</v>
-      </c>
-      <c r="G76">
-        <f t="shared" ca="1" si="41"/>
-        <v>9.0224246671338475E-3</v>
-      </c>
-      <c r="H76">
-        <f t="shared" ca="1" si="41"/>
-        <v>4.2342688007016007E-3</v>
-      </c>
-      <c r="I76">
-        <f t="shared" ca="1" si="41"/>
-        <v>8.688170591807815E-4</v>
-      </c>
-    </row>
-    <row r="77" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
-        <v>45</v>
-      </c>
-      <c r="C77" t="s">
-        <v>36</v>
-      </c>
-      <c r="D77">
-        <f t="shared" ref="D77:I83" ca="1" si="42">INDIRECT($B77&amp;D$74)</f>
-        <v>1</v>
-      </c>
-      <c r="E77">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.4340626178800453</v>
-      </c>
-      <c r="F77">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.24776074412195334</v>
-      </c>
-      <c r="G77">
-        <f t="shared" ca="1" si="42"/>
-        <v>8.3787208015378339E-2</v>
-      </c>
-      <c r="H77">
-        <f t="shared" ca="1" si="42"/>
-        <v>3.4201828536101105E-2</v>
-      </c>
-      <c r="I77">
-        <f t="shared" ca="1" si="42"/>
-        <v>9.6885714093263558E-3</v>
-      </c>
-    </row>
-    <row r="78" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>46</v>
-      </c>
-      <c r="C78" t="s">
-        <v>37</v>
-      </c>
-      <c r="D78">
-        <f t="shared" ca="1" si="42"/>
-        <v>1</v>
-      </c>
-      <c r="E78">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.5837386664148092</v>
-      </c>
-      <c r="F78">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.45768846267772506</v>
-      </c>
-      <c r="G78">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.18458442838370565</v>
-      </c>
-      <c r="H78">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.11894967282525019</v>
-      </c>
-      <c r="I78">
-        <f t="shared" ca="1" si="42"/>
-        <v>3.7441314553990614E-2</v>
-      </c>
-    </row>
-    <row r="79" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>47</v>
-      </c>
-      <c r="C79" t="s">
-        <v>38</v>
-      </c>
-      <c r="D79">
-        <f t="shared" ca="1" si="42"/>
-        <v>1</v>
-      </c>
-      <c r="E79">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.85587103802812114</v>
-      </c>
-      <c r="F79">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.65277056501869546</v>
-      </c>
-      <c r="G79">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.39882866208355372</v>
-      </c>
-      <c r="H79">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.24774814727215388</v>
-      </c>
-      <c r="I79">
-        <f t="shared" ca="1" si="42"/>
-        <v>7.6798413900972681E-2</v>
-      </c>
-    </row>
-    <row r="80" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>48</v>
-      </c>
-      <c r="C80" t="s">
-        <v>39</v>
-      </c>
-      <c r="D80">
-        <f t="shared" ca="1" si="42"/>
-        <v>1</v>
-      </c>
-      <c r="E80">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.74037112654474202</v>
-      </c>
-      <c r="F80">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.65561263492645938</v>
-      </c>
-      <c r="G80">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.42923494259316725</v>
-      </c>
-      <c r="H80">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.32590042332626529</v>
-      </c>
-      <c r="I80">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.1060471166639463</v>
-      </c>
-    </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
-        <v>49</v>
-      </c>
-      <c r="C81" t="s">
-        <v>40</v>
-      </c>
-      <c r="D81">
-        <f t="shared" ca="1" si="42"/>
-        <v>1</v>
-      </c>
-      <c r="E81">
-        <f t="shared" ca="1" si="42"/>
-        <v>1.0132435054235573</v>
-      </c>
-      <c r="F81">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.95654492427468973</v>
-      </c>
-      <c r="G81">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.66199233637468557</v>
-      </c>
-      <c r="H81">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.58051032249760937</v>
-      </c>
-      <c r="I81">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.25933464199128892</v>
-      </c>
-    </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>42</v>
-      </c>
-      <c r="C82" t="s">
-        <v>34</v>
-      </c>
-      <c r="D82">
-        <f t="shared" ca="1" si="42"/>
-        <v>1</v>
-      </c>
-      <c r="E82">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.91842711769462704</v>
-      </c>
-      <c r="F82">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.88553491141565022</v>
-      </c>
-      <c r="G82">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.55636291028423746</v>
-      </c>
-      <c r="H82">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.54508436162686269</v>
-      </c>
-      <c r="I82">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.3334187692711359</v>
-      </c>
-    </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
-        <v>43</v>
-      </c>
-      <c r="C83" t="s">
-        <v>41</v>
-      </c>
-      <c r="D83">
-        <f t="shared" ca="1" si="42"/>
-        <v>1</v>
-      </c>
-      <c r="E83">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.90940071715024406</v>
-      </c>
-      <c r="F83">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.75528135029279431</v>
-      </c>
-      <c r="G83">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.72884005664714269</v>
-      </c>
-      <c r="H83">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.69801573514423099</v>
-      </c>
-      <c r="I83">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.47433688703445515</v>
+      <c r="F84" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="G84" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="H84" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="I84" s="1">
+        <v>0.42</v>
       </c>
     </row>
   </sheetData>
@@ -22001,22 +20466,22 @@
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -22040,7 +20505,7 @@
         <v>7.7827453613281254E-5</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -22152,7 +20617,7 @@
         <v>0.19378960132598877</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -22198,7 +20663,7 @@
         <v>58.751106262207031</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">

</xml_diff>